<commit_message>
modified config of skill
Former-commit-id: fe040c676c9613e89d960a202e65bc82a7479a86 [formerly e77dc7235bc721b4b621df790351573ce62439c7]
Former-commit-id: 57b7027e3c0521d238989a7623c31108e8bc3eeb
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Skill.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Skill.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19560" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Skill" type="4" background="1" refreshedVersion="2" saveData="1">
-    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlFormat="all" htmlTables="1"/>
+  <connection id="1" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -88,14 +92,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -103,7 +101,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -155,23 +153,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -192,14 +175,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -498,6 +486,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -530,15 +519,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.875" customWidth="1"/>
     <col min="2" max="2" width="8.25" customWidth="1"/>
@@ -546,13 +534,11 @@
     <col min="4" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="8" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -610,7 +596,7 @@
         <v>60</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -619,7 +605,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -642,7 +628,7 @@
         <v>61</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -651,7 +637,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -673,8 +659,8 @@
       <c r="G4">
         <v>62</v>
       </c>
-      <c r="H4" s="4">
-        <v>3</v>
+      <c r="H4">
+        <v>2.5</v>
       </c>
       <c r="I4" s="3">
         <v>0</v>
@@ -683,7 +669,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -705,8 +691,8 @@
       <c r="G5">
         <v>63</v>
       </c>
-      <c r="H5" s="4">
-        <v>3</v>
+      <c r="H5">
+        <v>2.5</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
@@ -715,7 +701,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -737,8 +723,8 @@
       <c r="G6">
         <v>101</v>
       </c>
-      <c r="H6" s="4">
-        <v>3</v>
+      <c r="H6">
+        <v>2.5</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
@@ -747,7 +733,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -769,8 +755,8 @@
       <c r="G7">
         <v>102</v>
       </c>
-      <c r="H7" s="4">
-        <v>3</v>
+      <c r="H7">
+        <v>2.5</v>
       </c>
       <c r="I7" s="4">
         <v>0</v>
@@ -779,7 +765,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -801,8 +787,8 @@
       <c r="G8">
         <v>103</v>
       </c>
-      <c r="H8" s="4">
-        <v>3</v>
+      <c r="H8">
+        <v>2.5</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
@@ -811,7 +797,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -833,8 +819,8 @@
       <c r="G9">
         <v>104</v>
       </c>
-      <c r="H9" s="4">
-        <v>3</v>
+      <c r="H9">
+        <v>2.5</v>
       </c>
       <c r="I9" s="4">
         <v>0</v>
@@ -844,8 +830,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>